<commit_message>
integration of buffer time in attendance
</commit_message>
<xml_diff>
--- a/admin/users.xlsx
+++ b/admin/users.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\attendance system\admin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\BIG WORLD\attendance system\contactless_attendance\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282B183F-7885-4DF9-879C-182673F3D0CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1394DD-4D6C-4FE5-80B2-DABD612A4929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>s.no</t>
   </si>
@@ -101,6 +101,18 @@
   </si>
   <si>
     <t>pan number</t>
+  </si>
+  <si>
+    <t>aditya</t>
+  </si>
+  <si>
+    <t>employee</t>
+  </si>
+  <si>
+    <t>manufacturing</t>
+  </si>
+  <si>
+    <t>C1001</t>
   </si>
 </sst>
 </file>
@@ -463,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T15" sqref="T15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,6 +566,23 @@
         <v>26</v>
       </c>
     </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>